<commit_message>
update sum stats tables
</commit_message>
<xml_diff>
--- a/Output/All Data EDA/Tabular EDA/Financial_Summary_Statistics.xlsx
+++ b/Output/All Data EDA/Tabular EDA/Financial_Summary_Statistics.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G121"/>
+  <dimension ref="A1:G129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1102,328 +1102,328 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Accounts Payable (Balance Sheet)</t>
+          <t>Common Plus Preferred Stock</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>957,290,323.93</t>
+          <t>338,752,830.58</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>-237,651,171.00</t>
+          <t>-74,100.00</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>356,700,000.00</t>
+          <t>6,000,000.00</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>11,433,000,000.00</t>
+          <t>9,817,134,000.00</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>1,551,108,353.02</t>
+          <t>926,606,262.05</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Constructed for Altman's Z</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Accounts Payable (Cash Flow Statement)</t>
+          <t>EBIT</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>5,154,565.15</t>
+          <t>304,424,183.99</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>-321,769,000.00</t>
+          <t>-1,364,004,000.00</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>122,944,000.00</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1,789,652,000.00</t>
+          <t>4,334,000,000.00</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>82,110,968.91</t>
+          <t>556,409,802.60</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Constructed for Altman's Z</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Accounts Receivables</t>
+          <t>Ratio A</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>-11,478,236.25</t>
+          <t>0.02</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>-544,000,000.00</t>
+          <t>-0.02</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>0.02</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>325,000,000.00</t>
+          <t>0.08</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>91,535,961.30</t>
+          <t>0.02</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Constructed for Altman's Z</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Accumulated Other Comprehensive Income (Loss)</t>
+          <t>Ratio B</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>-404,483,300.22</t>
+          <t>0.21</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>-5,290,000,000.00</t>
+          <t>0.04</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>-77,514,000.00</t>
+          <t>0.18</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>431,595,000.00</t>
+          <t>0.70</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>874,353,108.41</t>
+          <t>0.15</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Constructed for Altman's Z</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Capital Expenditure</t>
+          <t>Ratio C</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>-192,514,484.47</t>
+          <t>1.87</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>-1,867,000,000.00</t>
+          <t>0.29</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>-60,129,000.00</t>
+          <t>1.42</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>412,700.00</t>
+          <t>8.06</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>310,057,440.27</t>
+          <t>1.55</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Constructed for Altman's Z</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Capital Lease Obligations</t>
+          <t>Ratio D</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>24,642,498.79</t>
+          <t>0.13</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>-0.13</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>0.10</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>9,056,234,000.00</t>
+          <t>0.57</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>228,328,885.18</t>
+          <t>0.15</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Constructed for Altman's Z</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Cash and Cash Equivalents</t>
+          <t>Ratio E</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>862,135,865.07</t>
+          <t>0.23</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>-0.74</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>333,000,000.00</t>
+          <t>0.21</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>9,223,000,000.00</t>
+          <t>1.01</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>1,366,595,243.17</t>
+          <t>0.32</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Constructed for Altman's Z</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Cash and Short Term Investments</t>
+          <t>Working Capital</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>1,060,086,810.64</t>
+          <t>1,125,108,587.77</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>-28,931,855,000.00</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>363,008,000.00</t>
+          <t>543,614,000.00</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>15,601,000,000.00</t>
+          <t>39,464,552,600.00</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>1,890,682,420.93</t>
+          <t>3,845,915,891.90</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Constructed for Altman's Z</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Cash at Beginning of Period</t>
+          <t>Accounts Payable (Balance Sheet)</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>867,410,489.82</t>
+          <t>957,290,323.93</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>-2,556,000.00</t>
+          <t>-237,651,171.00</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>334,000,000.00</t>
+          <t>356,700,000.00</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>9,610,000,000.00</t>
+          <t>11,433,000,000.00</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>1,388,834,800.13</t>
+          <t>1,551,108,353.02</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -1435,32 +1435,32 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Cash at End of Period</t>
+          <t>Accounts Payable (Cash Flow Statement)</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>871,017,693.39</t>
+          <t>5,154,565.15</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>-154,400.00</t>
+          <t>-321,769,000.00</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>335,469,000.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>9,743,000,000.00</t>
+          <t>1,789,652,000.00</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>1,394,641,397.30</t>
+          <t>82,110,968.91</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -1472,32 +1472,32 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Change in Working Capital</t>
+          <t>Accounts Receivables</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>-17,557,103.20</t>
+          <t>-11,478,236.25</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>-870,000,000.00</t>
+          <t>-544,000,000.00</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>-2,384,000.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>753,000,000.00</t>
+          <t>325,000,000.00</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>183,788,257.05</t>
+          <t>91,535,961.30</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -1509,32 +1509,32 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Common Stock</t>
+          <t>Accumulated Other Comprehensive Income (Loss)</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>329,277,684.36</t>
+          <t>-404,483,300.22</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>-539,800.00</t>
+          <t>-5,290,000,000.00</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>3,800,000.00</t>
+          <t>-77,514,000.00</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>9,817,134,000.00</t>
+          <t>431,595,000.00</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>925,626,949.20</t>
+          <t>874,353,108.41</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -1546,32 +1546,32 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Common Stock Issued</t>
+          <t>Capital Expenditure</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>44,672,509.36</t>
+          <t>-192,514,484.47</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>-3,572,000.00</t>
+          <t>-1,867,000,000.00</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>43,000.00</t>
+          <t>-60,129,000.00</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1,111,490,728.00</t>
+          <t>412,700.00</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>124,027,450.20</t>
+          <t>310,057,440.27</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -1583,32 +1583,32 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Common Stock Repurchased</t>
+          <t>Capital Lease Obligations</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>-78,527,033.90</t>
+          <t>24,642,498.79</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>-2,086,545,366.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>-773,000.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>545,656,614.52</t>
+          <t>9,056,234,000.00</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>188,219,352.34</t>
+          <t>228,328,885.18</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
@@ -1620,32 +1620,32 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Cost and Expenses</t>
+          <t>Cash and Cash Equivalents</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2,317,513,877.07</t>
+          <t>862,135,865.07</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>-2,495,000.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>1,121,064,000.00</t>
+          <t>333,000,000.00</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>22,769,000,000.00</t>
+          <t>9,223,000,000.00</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>3,357,899,606.58</t>
+          <t>1,366,595,243.17</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
@@ -1657,32 +1657,32 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Cost of Revenue</t>
+          <t>Cash and Short Term Investments</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>1,624,233,369.18</t>
+          <t>1,060,086,810.64</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>-3,094,000.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>787,700,000.00</t>
+          <t>363,008,000.00</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>18,303,000,000.00</t>
+          <t>15,601,000,000.00</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2,405,765,370.43</t>
+          <t>1,890,682,420.93</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
@@ -1694,32 +1694,32 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Debt Repayment</t>
+          <t>Cash at Beginning of Period</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>-247,880,234.24</t>
+          <t>867,410,489.82</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>-3,001,000,000.00</t>
+          <t>-2,556,000.00</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>-33,400,000.00</t>
+          <t>334,000,000.00</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>200.00</t>
+          <t>9,610,000,000.00</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>471,724,050.37</t>
+          <t>1,388,834,800.13</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
@@ -1731,32 +1731,32 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Deferred Income Tax</t>
+          <t>Cash at End of Period</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>6,154,669.54</t>
+          <t>871,017,693.39</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>-253,000,000.00</t>
+          <t>-154,400.00</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>64,000.00</t>
+          <t>335,469,000.00</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>1,850,454,000.00</t>
+          <t>9,743,000,000.00</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>58,927,713.28</t>
+          <t>1,394,641,397.30</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
@@ -1768,32 +1768,32 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Deferred Revenue</t>
+          <t>Change in Working Capital</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>310,000,739.66</t>
+          <t>-17,557,103.20</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>-116,912,000.00</t>
+          <t>-870,000,000.00</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>50,066,000.00</t>
+          <t>-2,384,000.00</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>4,918,100,000.00</t>
+          <t>753,000,000.00</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>642,489,899.31</t>
+          <t>183,788,257.05</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
@@ -1805,32 +1805,32 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Depreciation and Amortization (Cash Flow Statement)</t>
+          <t>Common Stock</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>141,811,048.14</t>
+          <t>329,277,684.36</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>-675,312.00</t>
+          <t>-539,800.00</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>53,551,000.00</t>
+          <t>3,800,000.00</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>1,529,000,000.00</t>
+          <t>9,817,134,000.00</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>210,315,836.18</t>
+          <t>925,626,949.20</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
@@ -1842,32 +1842,32 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Depreciation and Amortization (Income Statement)</t>
+          <t>Common Stock Issued</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>140,571,212.83</t>
+          <t>44,672,509.36</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>-1,550,000.00</t>
+          <t>-3,572,000.00</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>54,507,000.00</t>
+          <t>43,000.00</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>1,371,000,000.00</t>
+          <t>1,111,490,728.00</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>203,167,331.44</t>
+          <t>124,027,450.20</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
@@ -1879,32 +1879,32 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Diluted EPS</t>
+          <t>Common Stock Repurchased</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>0.51</t>
+          <t>-78,527,033.90</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>-156.36</t>
+          <t>-2,086,545,366.00</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>0.51</t>
+          <t>-773,000.00</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>49.73</t>
+          <t>545,656,614.52</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>3.31</t>
+          <t>188,219,352.34</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -1916,32 +1916,32 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Dividends Paid</t>
+          <t>Cost and Expenses</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>-91,357,096.76</t>
+          <t>2,317,513,877.07</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>-1,233,000,000.00</t>
+          <t>-2,495,000.00</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>-21,054,000.00</t>
+          <t>1,121,064,000.00</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>22,769,000,000.00</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>182,429,714.55</t>
+          <t>3,357,899,606.58</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
@@ -1953,32 +1953,32 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>EBITDA</t>
+          <t>Cost of Revenue</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>444,995,396.82</t>
+          <t>1,624,233,369.18</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>-66,200,000.00</t>
+          <t>-3,094,000.00</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>193,000,000.00</t>
+          <t>787,700,000.00</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>4,410,000,000.00</t>
+          <t>18,303,000,000.00</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>644,706,471.62</t>
+          <t>2,405,765,370.43</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
@@ -1990,32 +1990,32 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>EBITDA Ratio</t>
+          <t>Debt Repayment</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>0.20</t>
+          <t>-247,880,234.24</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>-5.77</t>
+          <t>-3,001,000,000.00</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>0.17</t>
+          <t>-33,400,000.00</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2.16</t>
+          <t>200.00</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>0.22</t>
+          <t>471,724,050.37</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
@@ -2027,32 +2027,32 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>EPS</t>
+          <t>Deferred Income Tax</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>0.52</t>
+          <t>6,154,669.54</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>-156.36</t>
+          <t>-253,000,000.00</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>0.52</t>
+          <t>64,000.00</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>53.75</t>
+          <t>1,850,454,000.00</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>3.33</t>
+          <t>58,927,713.28</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
@@ -2064,32 +2064,32 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Effect of Foreign Exchange Changes on Cash</t>
+          <t>Deferred Revenue</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>-1,697,085.83</t>
+          <t>310,000,739.66</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>-65,000,000.00</t>
+          <t>-116,912,000.00</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>50,066,000.00</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>52,000,000.00</t>
+          <t>4,918,100,000.00</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>11,200,007.88</t>
+          <t>642,489,899.31</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
@@ -2101,32 +2101,32 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Free Cash Flow</t>
+          <t>Depreciation and Amortization (Cash Flow Statement)</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>156,892,657.81</t>
+          <t>141,811,048.14</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>-541,000,000.00</t>
+          <t>-675,312.00</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>51,691,000.00</t>
+          <t>53,551,000.00</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2,683,000,000.00</t>
+          <t>1,529,000,000.00</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>389,666,937.19</t>
+          <t>210,315,836.18</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
@@ -2138,32 +2138,32 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>General and Administrative Expenses</t>
+          <t>Depreciation and Amortization (Income Statement)</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>153,933,016.99</t>
+          <t>140,571,212.83</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>-2,738,500.00</t>
+          <t>-1,550,000.00</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>33,768,000.00</t>
+          <t>54,507,000.00</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2,007,000,000.00</t>
+          <t>1,371,000,000.00</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>303,900,948.38</t>
+          <t>203,167,331.44</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
@@ -2175,32 +2175,32 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Goodwill</t>
+          <t>Diluted EPS</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>2,009,260,205.06</t>
+          <t>0.51</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>-202,702,100.00</t>
+          <t>-156.36</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>636,039,000.00</t>
+          <t>0.51</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>23,389,000,000.00</t>
+          <t>49.73</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>3,554,057,246.39</t>
+          <t>3.31</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
@@ -2212,32 +2212,32 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Goodwill and Intangible Assets</t>
+          <t>Dividends Paid</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>3,102,882,804.88</t>
+          <t>-91,357,096.76</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>-1,618,944,000.00</t>
+          <t>-1,233,000,000.00</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>970,000,000.00</t>
+          <t>-21,054,000.00</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>37,123,000,000.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>5,639,038,312.52</t>
+          <t>182,429,714.55</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
@@ -2249,32 +2249,32 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Gross Profit</t>
+          <t>EBITDA</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>861,821,178.07</t>
+          <t>444,995,396.82</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>-7,195,000.00</t>
+          <t>-66,200,000.00</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>378,500,000.00</t>
+          <t>193,000,000.00</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>9,223,000,000.00</t>
+          <t>4,410,000,000.00</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>1,365,410,717.45</t>
+          <t>644,706,471.62</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
@@ -2286,32 +2286,32 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Gross Profit Ratio</t>
+          <t>EBITDA Ratio</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>0.37</t>
+          <t>0.20</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>-5.65</t>
+          <t>-5.77</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>0.34</t>
+          <t>0.17</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>2.32</t>
+          <t>2.16</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>0.26</t>
+          <t>0.22</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
@@ -2323,32 +2323,32 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Income Before Tax</t>
+          <t>EPS</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>255,351,974.53</t>
+          <t>0.52</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>-353,153,000.00</t>
+          <t>-156.36</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>91,900,000.00</t>
+          <t>0.52</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>2,951,000,000.00</t>
+          <t>53.75</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>434,623,029.43</t>
+          <t>3.33</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
@@ -2360,32 +2360,32 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Income Before Tax Ratio</t>
+          <t>Effect of Foreign Exchange Changes on Cash</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>0.07</t>
+          <t>-1,697,085.83</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>-9.38</t>
+          <t>-65,000,000.00</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>0.09</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2.68</t>
+          <t>52,000,000.00</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>0.35</t>
+          <t>11,200,007.88</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
@@ -2397,32 +2397,32 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Income Tax Expense</t>
+          <t>Free Cash Flow</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>69,444,774.33</t>
+          <t>156,892,657.81</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>-119,131,000.00</t>
+          <t>-541,000,000.00</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>22,100,000.00</t>
+          <t>51,691,000.00</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>736,000,000.00</t>
+          <t>2,683,000,000.00</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>121,681,731.43</t>
+          <t>389,666,937.19</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
@@ -2434,32 +2434,32 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Intangible Assets</t>
+          <t>General and Administrative Expenses</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>835,940,509.51</t>
+          <t>153,933,016.99</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>-421,000.00</t>
+          <t>-2,738,500.00</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>170,197,000.00</t>
+          <t>33,768,000.00</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>14,110,100,000.00</t>
+          <t>2,007,000,000.00</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>1,785,542,119.17</t>
+          <t>303,900,948.38</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
@@ -2471,32 +2471,32 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Interest Expense</t>
+          <t>Goodwill</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>46,568,508.69</t>
+          <t>2,009,260,205.06</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>-16,400,000.00</t>
+          <t>-202,702,100.00</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>23,000,000.00</t>
+          <t>636,039,000.00</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>386,000,000.00</t>
+          <t>23,389,000,000.00</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>61,712,161.15</t>
+          <t>3,554,057,246.39</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
@@ -2508,32 +2508,32 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Interest Income</t>
+          <t>Goodwill and Intangible Assets</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>2,372,725.23</t>
+          <t>3,102,882,804.88</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>-62,900.00</t>
+          <t>-1,618,944,000.00</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>970,000,000.00</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>69,000,000.00</t>
+          <t>37,123,000,000.00</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>6,859,086.75</t>
+          <t>5,639,038,312.52</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
@@ -2545,32 +2545,32 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Inventory (Balance Sheet)</t>
+          <t>Gross Profit</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>933,043,177.40</t>
+          <t>861,821,178.07</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>-19,626,000.00</t>
+          <t>-7,195,000.00</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>403,789,000.00</t>
+          <t>378,500,000.00</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>8,328,000,000.00</t>
+          <t>9,223,000,000.00</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>1,398,934,358.21</t>
+          <t>1,365,410,717.45</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
@@ -2582,32 +2582,32 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Inventory (Cash Flow Statement)</t>
+          <t>Gross Profit Ratio</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>-10,302,495.14</t>
+          <t>0.37</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>-420,000,000.00</t>
+          <t>-5.65</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>0.34</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>289,000,000.00</t>
+          <t>2.32</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>70,374,129.32</t>
+          <t>0.26</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
@@ -2619,32 +2619,32 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Investments in Property, Plants, and Equipment</t>
+          <t>Income Before Tax</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>-193,897,744.95</t>
+          <t>255,351,974.53</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>-1,921,864,000.00</t>
+          <t>-353,153,000.00</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>-60,373,000.00</t>
+          <t>91,900,000.00</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>412,700.00</t>
+          <t>2,951,000,000.00</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>313,436,441.14</t>
+          <t>434,623,029.43</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
@@ -2656,32 +2656,32 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Long-Term Debt</t>
+          <t>Income Before Tax Ratio</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>4,159,473,460.27</t>
+          <t>0.07</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>-651,718.00</t>
+          <t>-9.38</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>1,822,139,000.00</t>
+          <t>0.09</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>31,359,000,000.00</t>
+          <t>2.68</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>5,574,538,232.32</t>
+          <t>0.35</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
@@ -2693,32 +2693,32 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Long-Term Investments</t>
+          <t>Income Tax Expense</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>494,196,440.41</t>
+          <t>69,444,774.33</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>-490,677,000.00</t>
+          <t>-119,131,000.00</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>12,449,000.00</t>
+          <t>22,100,000.00</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>10,981,000,000.00</t>
+          <t>736,000,000.00</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>1,359,571,399.50</t>
+          <t>121,681,731.43</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
@@ -2730,32 +2730,32 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Minority Interest</t>
+          <t>Intangible Assets</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>90,043,651.07</t>
+          <t>835,940,509.51</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>-20,252,654.04</t>
+          <t>-421,000.00</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>1,600,000.00</t>
+          <t>170,197,000.00</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>2,316,406,000.00</t>
+          <t>14,110,100,000.00</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>268,200,905.93</t>
+          <t>1,785,542,119.17</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
@@ -2767,32 +2767,32 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Net Acquisitions</t>
+          <t>Interest Expense</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>-32,878,764.18</t>
+          <t>46,568,508.69</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>-805,960,000.00</t>
+          <t>-16,400,000.00</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>23,000,000.00</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>249,000,000.00</t>
+          <t>386,000,000.00</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>116,107,004.20</t>
+          <t>61,712,161.15</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
@@ -2804,32 +2804,32 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Net Cash Provided by Operating Activities</t>
+          <t>Interest Income</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>352,446,106.81</t>
+          <t>2,372,725.23</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>-179,404,000.00</t>
+          <t>-62,900.00</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>143,626,000.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>3,870,000,000.00</t>
+          <t>69,000,000.00</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>545,602,564.63</t>
+          <t>6,859,086.75</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
@@ -2841,32 +2841,32 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Net Cash Used for Investing Activities</t>
+          <t>Inventory (Balance Sheet)</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>-252,575,304.44</t>
+          <t>933,043,177.40</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>-2,840,033,000.00</t>
+          <t>-19,626,000.00</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>-71,100,000.00</t>
+          <t>403,789,000.00</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>325,900,000.00</t>
+          <t>8,328,000,000.00</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>443,647,871.52</t>
+          <t>1,398,934,358.21</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
@@ -2878,32 +2878,32 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Net Cash Used or Provided by Financing Activities</t>
+          <t>Inventory (Cash Flow Statement)</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>-114,570,062.00</t>
+          <t>-10,302,495.14</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>-2,444,000,000.00</t>
+          <t>-420,000,000.00</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>-29,157,000.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>1,094,000,000.00</t>
+          <t>289,000,000.00</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>399,330,481.52</t>
+          <t>70,374,129.32</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
@@ -2915,32 +2915,32 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Net Change in Cash</t>
+          <t>Investments in Property, Plants, and Equipment</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>3,933,018.18</t>
+          <t>-193,897,744.95</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>-1,161,000,000.00</t>
+          <t>-1,921,864,000.00</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>573,000.00</t>
+          <t>-60,373,000.00</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>1,401,000,000.00</t>
+          <t>412,700.00</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>269,005,283.68</t>
+          <t>313,436,441.14</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
@@ -2952,32 +2952,32 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Net Debt</t>
+          <t>Long-Term Debt</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>3,597,141,664.59</t>
+          <t>4,159,473,460.27</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>-1,044,500,000.00</t>
+          <t>-651,718.00</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>1,508,594,000.00</t>
+          <t>1,822,139,000.00</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>30,761,000,000.00</t>
+          <t>31,359,000,000.00</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>5,338,457,121.62</t>
+          <t>5,574,538,232.32</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
@@ -2989,32 +2989,32 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Net Income (Cash Flow Statement)</t>
+          <t>Long-Term Investments</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>189,122,176.12</t>
+          <t>494,196,440.41</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>-327,000,000.00</t>
+          <t>-490,677,000.00</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>66,190,000.00</t>
+          <t>12,449,000.00</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>2,402,000,000.00</t>
+          <t>10,981,000,000.00</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>336,635,167.35</t>
+          <t>1,359,571,399.50</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
@@ -3026,32 +3026,32 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Net Income (Income Statement)</t>
+          <t>Minority Interest</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>185,944,828.27</t>
+          <t>90,043,651.07</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>-329,864,000.00</t>
+          <t>-20,252,654.04</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>66,389,000.00</t>
+          <t>1,600,000.00</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>2,340,000,000.00</t>
+          <t>2,316,406,000.00</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>330,952,161.49</t>
+          <t>268,200,905.93</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
@@ -3063,32 +3063,32 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Net Income Ratio</t>
+          <t>Net Acquisitions</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>0.05</t>
+          <t>-32,878,764.18</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>-8.88</t>
+          <t>-805,960,000.00</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>0.07</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>2.72</t>
+          <t>249,000,000.00</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>0.29</t>
+          <t>116,107,004.20</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
@@ -3100,32 +3100,32 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Net Property Plant Equipment</t>
+          <t>Net Cash Provided by Operating Activities</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>4,931,687,321.78</t>
+          <t>352,446,106.81</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>-179,404,000.00</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>1,389,600,000.00</t>
+          <t>143,626,000.00</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>44,441,000,000.00</t>
+          <t>3,870,000,000.00</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>7,885,938,319.99</t>
+          <t>545,602,564.63</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
@@ -3137,32 +3137,32 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Net Receivables</t>
+          <t>Net Cash Used for Investing Activities</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>1,276,905,848.63</t>
+          <t>-252,575,304.44</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>-4,199,600.00</t>
+          <t>-2,840,033,000.00</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>570,338,000.00</t>
+          <t>-71,100,000.00</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>12,116,000,000.00</t>
+          <t>325,900,000.00</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>1,776,578,353.43</t>
+          <t>443,647,871.52</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
@@ -3174,32 +3174,32 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Non-Current Deferred Revenue</t>
+          <t>Net Cash Used or Provided by Financing Activities</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>248,840,448.23</t>
+          <t>-114,570,062.00</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>-500,933,000.00</t>
+          <t>-2,444,000,000.00</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>-29,157,000.00</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>5,778,000,000.00</t>
+          <t>1,094,000,000.00</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>723,186,467.01</t>
+          <t>399,330,481.52</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
@@ -3211,32 +3211,32 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Non-Current Deferred Tax Liabilities</t>
+          <t>Net Change in Cash</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>702,874,797.74</t>
+          <t>3,933,018.18</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>-3,818,507.00</t>
+          <t>-1,161,000,000.00</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>135,597,000.00</t>
+          <t>573,000.00</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>8,306,000,000.00</t>
+          <t>1,401,000,000.00</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>1,400,029,509.57</t>
+          <t>269,005,283.68</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
@@ -3248,32 +3248,32 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Operating Cash Flow</t>
+          <t>Net Debt</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>352,446,106.81</t>
+          <t>3,597,141,664.59</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>-179,404,000.00</t>
+          <t>-1,044,500,000.00</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>143,626,000.00</t>
+          <t>1,508,594,000.00</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>3,870,000,000.00</t>
+          <t>30,761,000,000.00</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>545,602,564.63</t>
+          <t>5,338,457,121.62</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
@@ -3285,32 +3285,32 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Operating Expenses</t>
+          <t>Net Income (Cash Flow Statement)</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>538,189,512.49</t>
+          <t>189,122,176.12</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>-13,530,000.00</t>
+          <t>-327,000,000.00</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>221,700,000.00</t>
+          <t>66,190,000.00</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>6,252,000,000.00</t>
+          <t>2,402,000,000.00</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>918,426,909.60</t>
+          <t>336,635,167.35</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
@@ -3322,32 +3322,32 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Operating Income</t>
+          <t>Net Income (Income Statement)</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>302,231,079.76</t>
+          <t>185,944,828.27</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>-208,377,000.00</t>
+          <t>-329,864,000.00</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>122,000,000.00</t>
+          <t>66,389,000.00</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>3,294,000,000.00</t>
+          <t>2,340,000,000.00</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>475,077,278.15</t>
+          <t>330,952,161.49</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
@@ -3359,32 +3359,32 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Operating Income Ratio</t>
+          <t>Net Income Ratio</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>0.11</t>
+          <t>0.05</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>-9.71</t>
+          <t>-8.88</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>0.12</t>
+          <t>0.07</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>2.86</t>
+          <t>2.72</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>0.31</t>
+          <t>0.29</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
@@ -3396,32 +3396,32 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Other Assets</t>
+          <t>Net Property Plant Equipment</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>5,662.39</t>
+          <t>4,931,687,321.78</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>-19,834,700.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>1,389,600,000.00</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>8,948,000.00</t>
+          <t>44,441,000,000.00</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>421,776.93</t>
+          <t>7,885,938,319.99</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
@@ -3433,32 +3433,32 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Other Current Assets</t>
+          <t>Net Receivables</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>370,526,390.88</t>
+          <t>1,276,905,848.63</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>-98,000.00</t>
+          <t>-4,199,600.00</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>119,600,000.00</t>
+          <t>570,338,000.00</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>4,968,950,000.00</t>
+          <t>12,116,000,000.00</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>664,643,317.21</t>
+          <t>1,776,578,353.43</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
@@ -3470,32 +3470,32 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Other Current Liabilities</t>
+          <t>Non-Current Deferred Revenue</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>955,075,890.93</t>
+          <t>248,840,448.23</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>-48,317,000.00</t>
+          <t>-500,933,000.00</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>322,800,000.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>12,137,000,000.00</t>
+          <t>5,778,000,000.00</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>1,782,231,297.37</t>
+          <t>723,186,467.01</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
@@ -3507,32 +3507,32 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Other Expenses</t>
+          <t>Non-Current Deferred Tax Liabilities</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>50,749,806.82</t>
+          <t>702,874,797.74</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>-64,000,000.00</t>
+          <t>-3,818,507.00</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>585,000.00</t>
+          <t>135,597,000.00</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>16,189,674,590.00</t>
+          <t>8,306,000,000.00</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>342,110,629.66</t>
+          <t>1,400,029,509.57</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
@@ -3544,32 +3544,32 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Other Financing Activities</t>
+          <t>Operating Cash Flow</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>217,421,866.42</t>
+          <t>352,446,106.81</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>-975,168,999.00</t>
+          <t>-179,404,000.00</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>8,000,000.00</t>
+          <t>143,626,000.00</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>3,297,501,000.00</t>
+          <t>3,870,000,000.00</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>515,334,960.45</t>
+          <t>545,602,564.63</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
@@ -3581,32 +3581,32 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Other Investing Activities</t>
+          <t>Operating Expenses</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>4,573,739.09</t>
+          <t>538,189,512.49</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>-448,000,000.00</t>
+          <t>-13,530,000.00</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>106,000.00</t>
+          <t>221,700,000.00</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>3,060,433,659.00</t>
+          <t>6,252,000,000.00</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>96,736,267.62</t>
+          <t>918,426,909.60</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
@@ -3618,32 +3618,32 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Other Liabilities</t>
+          <t>Operating Income</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>95,902.58</t>
+          <t>302,231,079.76</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>-3,063,000.00</t>
+          <t>-208,377,000.00</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>122,000,000.00</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>51,076,000.00</t>
+          <t>3,294,000,000.00</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>1,967,227.53</t>
+          <t>475,077,278.15</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
@@ -3655,32 +3655,32 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Other Non-Cash Items</t>
+          <t>Operating Income Ratio</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>15,325,139.75</t>
+          <t>0.11</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>-1,848,719,007.00</t>
+          <t>-9.71</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>1,621,000.00</t>
+          <t>0.12</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>703,000,000.00</t>
+          <t>2.86</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>109,294,805.79</t>
+          <t>0.31</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
@@ -3692,32 +3692,32 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Other Non-Current Assets</t>
+          <t>Other Assets</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>506,778,121.04</t>
+          <t>5,662.39</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>-75,012,534,818.00</t>
+          <t>-19,834,700.00</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>158,696,000.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>8,037,000,000.00</t>
+          <t>8,948,000.00</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>1,778,143,597.09</t>
+          <t>421,776.93</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
@@ -3729,32 +3729,32 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Other Non-Current Liabilities</t>
+          <t>Other Current Assets</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>975,892,048.39</t>
+          <t>370,526,390.88</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>-286,041,895.00</t>
+          <t>-98,000.00</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>327,700,000.00</t>
+          <t>119,600,000.00</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>11,890,564,000.00</t>
+          <t>4,968,950,000.00</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>1,686,827,873.95</t>
+          <t>664,643,317.21</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
@@ -3766,32 +3766,32 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Other Total Stockholders' Equity</t>
+          <t>Other Current Liabilities</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>1,135,331,510.72</t>
+          <t>955,075,890.93</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>-12,393,000,000.00</t>
+          <t>-48,317,000.00</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>427,000,000.00</t>
+          <t>322,800,000.00</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>34,030,400,000.00</t>
+          <t>12,137,000,000.00</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>3,586,435,863.55</t>
+          <t>1,782,231,297.37</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
@@ -3803,32 +3803,32 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Other Working Capital</t>
+          <t>Other Expenses</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>21,414,823.22</t>
+          <t>50,749,806.82</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>-1,788,851,160.00</t>
+          <t>-64,000,000.00</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>585,000.00</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>40,341,689,407.00</t>
+          <t>16,189,674,590.00</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>786,599,061.35</t>
+          <t>342,110,629.66</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
@@ -3840,32 +3840,32 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Preferred Stock</t>
+          <t>Other Financing Activities</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>9,475,146.22</t>
+          <t>217,421,866.42</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>-975,168,999.00</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>8,000,000.00</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>401,500,000.00</t>
+          <t>3,297,501,000.00</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>42,785,110.93</t>
+          <t>515,334,960.45</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
@@ -3877,32 +3877,32 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Purchases of Investments</t>
+          <t>Other Investing Activities</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>-104,151,034.82</t>
+          <t>4,573,739.09</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>-11,997,654,000.00</t>
+          <t>-448,000,000.00</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>106,000.00</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>81,823,000.00</t>
+          <t>3,060,433,659.00</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>346,711,949.30</t>
+          <t>96,736,267.62</t>
         </is>
       </c>
       <c r="G94" t="inlineStr">
@@ -3914,17 +3914,17 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Research and Development Expenses</t>
+          <t>Other Liabilities</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>28,169,938.85</t>
+          <t>95,902.58</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>-214,000.00</t>
+          <t>-3,063,000.00</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -3934,12 +3934,12 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>893,000,000.00</t>
+          <t>51,076,000.00</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>94,071,513.75</t>
+          <t>1,967,227.53</t>
         </is>
       </c>
       <c r="G95" t="inlineStr">
@@ -3951,32 +3951,32 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Retained Earnings</t>
+          <t>Other Non-Cash Items</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>3,628,393,969.72</t>
+          <t>15,325,139.75</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>-4,839,000,000.00</t>
+          <t>-1,848,719,007.00</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>1,293,100,000.00</t>
+          <t>1,621,000.00</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>37,899,000,000.00</t>
+          <t>703,000,000.00</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>6,424,744,717.89</t>
+          <t>109,294,805.79</t>
         </is>
       </c>
       <c r="G96" t="inlineStr">
@@ -3988,32 +3988,32 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Revenue</t>
+          <t>Other Non-Current Assets</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>2,728,749,857.76</t>
+          <t>506,778,121.04</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>-4,273,000.00</t>
+          <t>-75,012,534,818.00</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>1,297,700,000.00</t>
+          <t>158,696,000.00</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>25,420,000,000.00</t>
+          <t>8,037,000,000.00</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>3,959,362,594.26</t>
+          <t>1,778,143,597.09</t>
         </is>
       </c>
       <c r="G97" t="inlineStr">
@@ -4025,32 +4025,32 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Sales and Maturities of Investments</t>
+          <t>Other Non-Current Liabilities</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>99,796,411.86</t>
+          <t>975,892,048.39</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>-9,409,000.00</t>
+          <t>-286,041,895.00</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>327,700,000.00</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>8,936,406,000.00</t>
+          <t>11,890,564,000.00</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>311,292,561.88</t>
+          <t>1,686,827,873.95</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
@@ -4062,32 +4062,32 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Selling General and Administrative Expenses</t>
+          <t>Other Total Stockholders' Equity</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>296,899,615.00</t>
+          <t>1,135,331,510.72</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>-5,054,000.00</t>
+          <t>-12,393,000,000.00</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>119,600,000.00</t>
+          <t>427,000,000.00</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>3,343,000,000.00</t>
+          <t>34,030,400,000.00</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>486,131,457.73</t>
+          <t>3,586,435,863.55</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
@@ -4099,17 +4099,17 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Selling and Marketing Expenses</t>
+          <t>Other Working Capital</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>25,431,647.83</t>
+          <t>21,414,823.22</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>-3,003,000.00</t>
+          <t>-1,788,851,160.00</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -4119,12 +4119,12 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>876,761,000.00</t>
+          <t>40,341,689,407.00</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>97,367,023.08</t>
+          <t>786,599,061.35</t>
         </is>
       </c>
       <c r="G100" t="inlineStr">
@@ -4136,17 +4136,17 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Short Term Investments</t>
+          <t>Preferred Stock</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>182,988,242.55</t>
+          <t>9,475,146.22</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>-515,000.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -4156,12 +4156,12 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>6,178,000,000.00</t>
+          <t>401,500,000.00</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>599,747,024.65</t>
+          <t>42,785,110.93</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
@@ -4173,32 +4173,32 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Short-Term Debt</t>
+          <t>Purchases of Investments</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>465,870,869.02</t>
+          <t>-104,151,034.82</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>-655,561.00</t>
+          <t>-11,997,654,000.00</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>83,800,000.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>5,363,000,000.00</t>
+          <t>81,823,000.00</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>885,210,679.51</t>
+          <t>346,711,949.30</t>
         </is>
       </c>
       <c r="G102" t="inlineStr">
@@ -4210,32 +4210,32 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Stock-Based Compensation</t>
+          <t>Research and Development Expenses</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>14,496,292.55</t>
+          <t>28,169,938.85</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>-36,000,000.00</t>
+          <t>-214,000.00</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>5,106,000.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>254,000,000.00</t>
+          <t>893,000,000.00</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>29,968,462.79</t>
+          <t>94,071,513.75</t>
         </is>
       </c>
       <c r="G103" t="inlineStr">
@@ -4247,32 +4247,32 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Tax Assets</t>
+          <t>Retained Earnings</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>378,132,518.58</t>
+          <t>3,628,393,969.72</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>-2,310,712,000.00</t>
+          <t>-4,839,000,000.00</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>48,963,000.00</t>
+          <t>1,293,100,000.00</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>6,535,000,000.00</t>
+          <t>37,899,000,000.00</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>909,237,680.35</t>
+          <t>6,424,744,717.89</t>
         </is>
       </c>
       <c r="G104" t="inlineStr">
@@ -4284,32 +4284,32 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Tax Payable</t>
+          <t>Revenue</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>60,670,669.07</t>
+          <t>2,728,749,857.76</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>-87,400.00</t>
+          <t>-4,273,000.00</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>2,810,000.00</t>
+          <t>1,297,700,000.00</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>1,187,000,000.00</t>
+          <t>25,420,000,000.00</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>150,628,980.40</t>
+          <t>3,959,362,594.26</t>
         </is>
       </c>
       <c r="G105" t="inlineStr">
@@ -4321,32 +4321,32 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Total Assets</t>
+          <t>Sales and Maturities of Investments</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>15,592,495,985.55</t>
+          <t>99,796,411.86</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>123,279.00</t>
+          <t>-9,409,000.00</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>7,048,475,000.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>131,119,000,000.00</t>
+          <t>8,936,406,000.00</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>21,911,032,910.64</t>
+          <t>311,292,561.88</t>
         </is>
       </c>
       <c r="G106" t="inlineStr">
@@ -4358,32 +4358,32 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Total Current Assets</t>
+          <t>Selling General and Administrative Expenses</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>3,937,085,272.11</t>
+          <t>296,899,615.00</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>29,954.00</t>
+          <t>-5,054,000.00</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>1,933,750,000.00</t>
+          <t>119,600,000.00</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>41,276,000,000.00</t>
+          <t>3,343,000,000.00</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>5,729,273,613.69</t>
+          <t>486,131,457.73</t>
         </is>
       </c>
       <c r="G107" t="inlineStr">
@@ -4395,32 +4395,32 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Total Current Liabilities</t>
+          <t>Selling and Marketing Expenses</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>2,811,976,684.34</t>
+          <t>25,431,647.83</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>24,083.00</t>
+          <t>-3,003,000.00</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>1,138,200,000.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>29,919,000,000.00</t>
+          <t>876,761,000.00</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>4,247,045,840.39</t>
+          <t>97,367,023.08</t>
         </is>
       </c>
       <c r="G108" t="inlineStr">
@@ -4432,32 +4432,32 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Total Debt</t>
+          <t>Short Term Investments</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>4,593,265,532.66</t>
+          <t>182,988,242.55</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
+          <t>-515,000.00</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="D109" t="inlineStr">
-        <is>
-          <t>2,019,244,000.00</t>
-        </is>
-      </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>37,124,000,000.00</t>
+          <t>6,178,000,000.00</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>6,254,194,800.16</t>
+          <t>599,747,024.65</t>
         </is>
       </c>
       <c r="G109" t="inlineStr">
@@ -4469,32 +4469,32 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Total Equity</t>
+          <t>Short-Term Debt</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>4,968,502,543.29</t>
+          <t>465,870,869.02</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>-501,467,000.00</t>
+          <t>-655,561.00</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>2,095,000,000.00</t>
+          <t>83,800,000.00</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>49,975,000,000.00</t>
+          <t>5,363,000,000.00</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>7,272,421,518.55</t>
+          <t>885,210,679.51</t>
         </is>
       </c>
       <c r="G110" t="inlineStr">
@@ -4506,32 +4506,32 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Total Investments</t>
+          <t>Stock-Based Compensation</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>729,199,594.64</t>
+          <t>14,496,292.55</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>-334,673,000.00</t>
+          <t>-36,000,000.00</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>43,275,000.00</t>
+          <t>5,106,000.00</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>19,331,000,000.00</t>
+          <t>254,000,000.00</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>1,944,649,108.26</t>
+          <t>29,968,462.79</t>
         </is>
       </c>
       <c r="G111" t="inlineStr">
@@ -4543,32 +4543,32 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Total Liabilities</t>
+          <t>Tax Assets</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>9,817,545,124.72</t>
+          <t>378,132,518.58</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>79,283.00</t>
+          <t>-2,310,712,000.00</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>4,308,693,000.00</t>
+          <t>48,963,000.00</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>87,293,000,000.00</t>
+          <t>6,535,000,000.00</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>13,527,062,565.42</t>
+          <t>909,237,680.35</t>
         </is>
       </c>
       <c r="G112" t="inlineStr">
@@ -4580,32 +4580,32 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Total Liabilities and Stockholders' Equity</t>
+          <t>Tax Payable</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>15,556,696,866.65</t>
+          <t>60,670,669.07</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>123,279.00</t>
+          <t>-87,400.00</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>7,043,426,000.00</t>
+          <t>2,810,000.00</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>131,119,000,000.00</t>
+          <t>1,187,000,000.00</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>21,905,884,302.05</t>
+          <t>150,628,980.40</t>
         </is>
       </c>
       <c r="G113" t="inlineStr">
@@ -4617,12 +4617,12 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Total Liabilities and Total Equity</t>
+          <t>Total Assets</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>15,556,696,866.65</t>
+          <t>15,592,495,985.55</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -4632,7 +4632,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>7,043,426,000.00</t>
+          <t>7,048,475,000.00</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
@@ -4642,7 +4642,7 @@
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>21,905,884,302.05</t>
+          <t>21,911,032,910.64</t>
         </is>
       </c>
       <c r="G114" t="inlineStr">
@@ -4654,32 +4654,32 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Total Non-Current Assets</t>
+          <t>Total Current Assets</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>11,011,964,229.49</t>
+          <t>3,937,085,272.11</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>49,861.00</t>
+          <t>29,954.00</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>4,119,200,000.00</t>
+          <t>1,933,750,000.00</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>104,263,000,000.00</t>
+          <t>41,276,000,000.00</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>15,994,777,583.25</t>
+          <t>5,729,273,613.69</t>
         </is>
       </c>
       <c r="G115" t="inlineStr">
@@ -4691,32 +4691,32 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Total Non-Current Liabilities</t>
+          <t>Total Current Liabilities</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>6,639,451,321.63</t>
+          <t>2,811,976,684.34</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>53,696.00</t>
+          <t>24,083.00</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>2,809,300,000.00</t>
+          <t>1,138,200,000.00</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>54,300,000,000.00</t>
+          <t>29,919,000,000.00</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>9,424,654,097.47</t>
+          <t>4,247,045,840.39</t>
         </is>
       </c>
       <c r="G116" t="inlineStr">
@@ -4728,32 +4728,32 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Total Other Income Expenses Net</t>
+          <t>Total Debt</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>-13,134,652.92</t>
+          <t>4,593,265,532.66</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>-503,976,000.00</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>-920,000.00</t>
+          <t>2,019,244,000.00</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>286,000,000.00</t>
+          <t>37,124,000,000.00</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>72,414,124.07</t>
+          <t>6,254,194,800.16</t>
         </is>
       </c>
       <c r="G117" t="inlineStr">
@@ -4765,32 +4765,32 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Total Stockholders' Equity</t>
+          <t>Total Equity</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>4,933,321,107.00</t>
+          <t>4,968,502,543.29</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>-526,491,000.00</t>
+          <t>-501,467,000.00</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>2,088,608,000.00</t>
+          <t>2,095,000,000.00</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>49,269,000,000.00</t>
+          <t>49,975,000,000.00</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>7,194,176,771.15</t>
+          <t>7,272,421,518.55</t>
         </is>
       </c>
       <c r="G118" t="inlineStr">
@@ -4802,32 +4802,32 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Weighted Average Shares Outstanding</t>
+          <t>Total Investments</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>352,790,171.17</t>
+          <t>729,199,594.64</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>-334,673,000.00</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>146,000,000.00</t>
+          <t>43,275,000.00</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>13,751,391,147.00</t>
+          <t>19,331,000,000.00</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>720,460,888.99</t>
+          <t>1,944,649,108.26</t>
         </is>
       </c>
       <c r="G119" t="inlineStr">
@@ -4839,32 +4839,32 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Weighted Average Shares Outstanding (Diluted)</t>
+          <t>Total Liabilities</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>316,630,108.94</t>
+          <t>9,817,545,124.72</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>79,283.00</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>145,951,913.00</t>
+          <t>4,308,693,000.00</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>13,986,214,405.00</t>
+          <t>87,293,000,000.00</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>547,337,219.46</t>
+          <t>13,527,062,565.42</t>
         </is>
       </c>
       <c r="G120" t="inlineStr">
@@ -4876,35 +4876,331 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
+          <t>Total Liabilities and Stockholders' Equity</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>15,556,696,866.65</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>123,279.00</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>7,043,426,000.00</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>131,119,000,000.00</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>21,905,884,302.05</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>Total Liabilities and Total Equity</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>15,556,696,866.65</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>123,279.00</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>7,043,426,000.00</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>131,119,000,000.00</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>21,905,884,302.05</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>Total Non-Current Assets</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>11,011,964,229.49</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>49,861.00</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>4,119,200,000.00</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>104,263,000,000.00</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>15,994,777,583.25</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>Total Non-Current Liabilities</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>6,639,451,321.63</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>53,696.00</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>2,809,300,000.00</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>54,300,000,000.00</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>9,424,654,097.47</t>
+        </is>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>Total Other Income Expenses Net</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>-13,134,652.92</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>-503,976,000.00</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>-920,000.00</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>286,000,000.00</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>72,414,124.07</t>
+        </is>
+      </c>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>Total Stockholders' Equity</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>4,933,321,107.00</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>-526,491,000.00</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>2,088,608,000.00</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>49,269,000,000.00</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>7,194,176,771.15</t>
+        </is>
+      </c>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>Weighted Average Shares Outstanding</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>352,790,171.17</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>146,000,000.00</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>13,751,391,147.00</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>720,460,888.99</t>
+        </is>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>Weighted Average Shares Outstanding (Diluted)</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>316,630,108.94</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>145,951,913.00</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>13,986,214,405.00</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>547,337,219.46</t>
+        </is>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
           <t>Market Capitalization</t>
         </is>
       </c>
-      <c r="B121" t="inlineStr">
+      <c r="B129" t="inlineStr">
         <is>
           <t>18,996,749,034.57</t>
         </is>
       </c>
-      <c r="C121" t="inlineStr">
+      <c r="C129" t="inlineStr">
         <is>
           <t>106,422.00</t>
         </is>
       </c>
-      <c r="D121" t="inlineStr">
+      <c r="D129" t="inlineStr">
         <is>
           <t>6,409,459,125.00</t>
         </is>
       </c>
-      <c r="E121" t="inlineStr">
+      <c r="E129" t="inlineStr">
         <is>
           <t>726,320,349,360.00</t>
         </is>
       </c>
-      <c r="F121" t="inlineStr">
+      <c r="F129" t="inlineStr">
         <is>
           <t>44,246,873,159.19</t>
         </is>
       </c>
-      <c r="G121" t="inlineStr">
+      <c r="G129" t="inlineStr">
         <is>
           <t>Market Capitalization</t>
         </is>

</xml_diff>